<commit_message>
done with upload parcelle
</commit_message>
<xml_diff>
--- a/apps/static/assets/template/Farm_Upload_template.xlsx
+++ b/apps/static/assets/template/Farm_Upload_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WORK\Python_dev\s-tim\apps\static\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2D9801-AC7F-449F-91D4-CAFE6A4B2BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1F6539-CEF9-4040-BE9C-1888A7E06DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1ADBAEC9-2E84-42B3-AEB4-6C807F91EDB2}"/>
   </bookViews>
@@ -25,31 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Surface</t>
-  </si>
-  <si>
-    <t>plants</t>
-  </si>
-  <si>
-    <t>Plants Productive</t>
-  </si>
-  <si>
-    <t>Age Moyen</t>
-  </si>
-  <si>
-    <t>Production estimee</t>
-  </si>
-  <si>
-    <t>Production estimee vrac</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>inspected</t>
   </si>
@@ -61,6 +37,33 @@
   </si>
   <si>
     <t>0.97 Ha</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>overallSize</t>
+  </si>
+  <si>
+    <t>totalPlants</t>
+  </si>
+  <si>
+    <t>productivePlants</t>
+  </si>
+  <si>
+    <t>averageAge</t>
+  </si>
+  <si>
+    <t>estimatedProduction</t>
+  </si>
+  <si>
+    <t>estimated_VRAC</t>
+  </si>
+  <si>
+    <t>farmerId</t>
   </si>
 </sst>
 </file>
@@ -451,87 +454,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{818C7251-4CB5-4160-9F9C-72E591436C7A}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>231</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E2" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2500</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2000</v>
-      </c>
-      <c r="F2" s="3">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>700</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>175</v>
       </c>
-      <c r="I2" s="3" t="b">
+      <c r="J2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>